<commit_message>
750 last non-tied games
</commit_message>
<xml_diff>
--- a/pred tool.xlsx
+++ b/pred tool.xlsx
@@ -49,8 +49,8 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Die elf häufigsten W scores der letzten 500 non tied RS games
-results |&gt; filter(Result == "W", Week &lt; 30) |&gt; tail(500) |&gt; pull(PF) |&gt; table() |&gt; sort(decreasing = T) |&gt; t() |&gt; t() |&gt; head(11)</t>
+          <t>Die elf häufigsten W scores der letzten 750 non tied RS games
+results |&gt; filter(Result == "W", Week &lt; 30) |&gt; tail(750) |&gt; pull(PF) |&gt; table() |&gt; sort(decreasing = T) |&gt; t() |&gt; t() |&gt; head(11)</t>
         </r>
       </text>
     </comment>
@@ -79,24 +79,6 @@
     <t>LAR</t>
   </si>
   <si>
-    <t xml:space="preserve">  24   26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  14   22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  9    20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  23   18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  21   17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  17   21</t>
-  </si>
-  <si>
     <t>Fav</t>
   </si>
   <si>
@@ -139,58 +121,76 @@
     <t>@ data table</t>
   </si>
   <si>
-    <t xml:space="preserve">  27   44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  20   40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  24   34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  31   32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  23   24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  19   20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  34   18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  37   17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  10   56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  16   38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  20   34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  3    21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  21   16</t>
-  </si>
-  <si>
     <t>MIA</t>
   </si>
   <si>
     <t>DAL</t>
   </si>
   <si>
-    <t xml:space="preserve">  30   27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  17   53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  13   33</t>
+    <t xml:space="preserve">  27   68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  20   56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  31   48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  24   46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  23   39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  30   39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  34   36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  17   30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  19   29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  28   27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  26   26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  17   80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  10   65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  16   56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  20   46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  13   44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  24   41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  14   38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3    33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7    28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  21   27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9    25</t>
   </si>
 </sst>
 </file>
@@ -647,29 +647,29 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3">
         <f>Q28</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3">
         <f>X28</f>
@@ -677,36 +677,36 @@
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="12"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="X1" s="12"/>
     </row>
@@ -715,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C2" s="6">
         <v>-13</v>
@@ -748,7 +748,7 @@
         <v>17</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M2" s="4">
         <f>VALUE(LEFT(L2,FIND("   ",L2,1)-1))</f>
@@ -756,11 +756,11 @@
       </c>
       <c r="N2" s="4">
         <f t="shared" ref="N2:N12" si="0">MATCH(P2,M$2:M$12,0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O2" s="4">
         <f>VALUE(RIGHT(L2,LEN(L2)-FIND("   ",L2,1)))</f>
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="P2" s="4">
         <f>SMALL(M$2:M$12,ROW()-1)</f>
@@ -768,14 +768,14 @@
       </c>
       <c r="Q2" s="4">
         <f t="shared" ref="Q2:Q12" si="1">INDEX(O$2:O$12,$N2)</f>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T2" s="4">
         <f>VALUE(LEFT(S2,FIND("   ",S2,1)-1))</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="U2" s="4">
         <f t="shared" ref="U2:U12" si="2">MATCH(W2,T$2:T$12,0)</f>
@@ -783,7 +783,7 @@
       </c>
       <c r="V2" s="4">
         <f>VALUE(RIGHT(S2,LEN(S2)-FIND("   ",S2,1)))</f>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="W2" s="4">
         <f>SMALL(T$2:T$12,ROW()-1)</f>
@@ -791,7 +791,7 @@
       </c>
       <c r="X2" s="4">
         <f t="shared" ref="X2:X12" si="3">INDEX(V$2:V$12,$N2)</f>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3:M12" si="8">VALUE(LEFT(L3,FIND("   ",L3,1)-1))</f>
@@ -838,11 +838,11 @@
       </c>
       <c r="N3" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3:O12" si="9">VALUE(RIGHT(L3,LEN(L3)-FIND("   ",L3,1)))</f>
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" ref="P3:P12" si="10">SMALL(M$2:M$12,ROW()-1)</f>
@@ -850,14 +850,14 @@
       </c>
       <c r="Q3" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" ref="T3:T12" si="11">VALUE(LEFT(S3,FIND("   ",S3,1)-1))</f>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="2"/>
@@ -865,15 +865,15 @@
       </c>
       <c r="V3" s="4">
         <f t="shared" ref="V3:V12" si="12">VALUE(RIGHT(S3,LEN(S3)-FIND("   ",S3,1)))</f>
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="W3" s="4">
         <f t="shared" ref="W3:W12" si="13">SMALL(T$2:T$12,ROW()-1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="X3" s="4">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -912,11 +912,11 @@
         <v>21</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
@@ -924,7 +924,7 @@
       </c>
       <c r="O4" s="4">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="10"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>35</v>
@@ -943,19 +943,19 @@
       </c>
       <c r="U4" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V4" s="4">
         <f t="shared" si="12"/>
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X4" s="4">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6">
         <v>-6</v>
@@ -980,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="7" t="str">
         <f t="shared" si="6"/>
@@ -994,27 +994,27 @@
         <v>20</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="10"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="S5" s="10" t="s">
         <v>36</v>
@@ -1025,47 +1025,47 @@
       </c>
       <c r="U5" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V5" s="4">
         <f t="shared" si="12"/>
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="W5" s="4">
         <f t="shared" si="13"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="L6" s="10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O6" s="4">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" si="10"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="T6" s="4">
         <f t="shared" si="11"/>
@@ -1073,47 +1073,47 @@
       </c>
       <c r="U6" s="4">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V6" s="4">
         <f t="shared" si="12"/>
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="W6" s="4">
         <f t="shared" si="13"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X6" s="4">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="L7" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="10"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="T7" s="4">
         <f t="shared" si="11"/>
@@ -1121,28 +1121,28 @@
       </c>
       <c r="U7" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="V7" s="4">
         <f t="shared" si="12"/>
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="W7" s="4">
         <f t="shared" si="13"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="X7" s="4">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="L8" s="10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="0"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="O8" s="4">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="10"/>
@@ -1158,10 +1158,10 @@
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="11"/>
@@ -1169,19 +1169,19 @@
       </c>
       <c r="U8" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1190,30 +1190,30 @@
         <v>MIA 30-17</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="10"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="T9" s="4">
         <f t="shared" si="11"/>
@@ -1221,19 +1221,19 @@
       </c>
       <c r="U9" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V9" s="4">
         <f t="shared" si="12"/>
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="W9" s="4">
         <f t="shared" si="13"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="X9" s="4">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -1246,50 +1246,50 @@
         <v>MIA 30-17, KC  27-20</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="8"/>
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" si="10"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="T10" s="4">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="U10" s="4">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="V10" s="4">
         <f t="shared" si="12"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="W10" s="4">
         <f t="shared" si="13"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X10" s="4">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -1302,34 +1302,34 @@
         <v>MIA 30-17, KC  27-20, MIN 23-21</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="10"/>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="T11" s="4">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" si="2"/>
@@ -1337,55 +1337,55 @@
       </c>
       <c r="V11" s="4">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W11" s="4">
         <f t="shared" si="13"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X11" s="4">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>DAL 27-20</v>
+        <v>DAL 26-20</v>
       </c>
       <c r="C12" s="11" t="str">
         <f>C11&amp;", "&amp;B12</f>
-        <v>MIA 30-17, KC  27-20, MIN 23-21, DAL 27-20</v>
+        <v>MIA 30-17, KC  27-20, MIN 23-21, DAL 26-20</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="8"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O12" s="4">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" si="10"/>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="T12" s="4">
         <f t="shared" si="11"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="U12" s="4">
         <f t="shared" si="2"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="V12" s="4">
         <f t="shared" si="12"/>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="W12" s="4">
         <f t="shared" si="13"/>
@@ -1401,29 +1401,29 @@
       </c>
       <c r="X12" s="4">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="M14" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N14" s="4">
         <v>21</v>
       </c>
       <c r="O14" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="T14" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="U14" s="4">
         <v>21</v>
       </c>
       <c r="V14" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="U17" s="4">
         <f t="shared" si="19"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V17" s="4">
         <f t="shared" si="20"/>
@@ -1503,19 +1503,19 @@
       </c>
       <c r="O18" s="4">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="19"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V18" s="4">
         <f t="shared" si="20"/>
@@ -1533,23 +1533,23 @@
     <row r="19" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N19" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O19" s="4">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="4">
         <f t="shared" si="17"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="4">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="V19" s="4">
         <f t="shared" si="20"/>
@@ -1567,7 +1567,7 @@
     <row r="20" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N20" s="4">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O20" s="4">
         <f t="shared" si="16"/>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="U20" s="4">
         <f t="shared" si="19"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V20" s="4">
         <f t="shared" si="20"/>
@@ -1601,7 +1601,7 @@
     <row r="21" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N21" s="4">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="16"/>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="U21" s="4">
         <f t="shared" si="19"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="20"/>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="U22" s="4">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V22" s="4">
         <f t="shared" si="20"/>
@@ -1669,7 +1669,7 @@
     <row r="23" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N23" s="4">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O23" s="4">
         <f t="shared" si="16"/>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="U23" s="4">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V23" s="4">
         <f t="shared" si="20"/>
@@ -1703,7 +1703,7 @@
     <row r="24" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N24" s="4">
         <f t="shared" si="15"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O24" s="4">
         <f t="shared" si="16"/>
@@ -1719,25 +1719,25 @@
       </c>
       <c r="U24" s="4">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="4">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="4">
         <f t="shared" si="21"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="X24" s="4">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N25" s="4">
         <f t="shared" si="15"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="16"/>
@@ -1753,25 +1753,25 @@
       </c>
       <c r="U25" s="4">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="4">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="X25" s="4">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N26" s="4">
         <f t="shared" si="15"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O26" s="4">
         <f t="shared" si="16"/>
@@ -1804,14 +1804,14 @@
     </row>
     <row r="28" spans="14:24" x14ac:dyDescent="0.2">
       <c r="P28" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q28" s="4">
         <f>SUMPRODUCT(P2:P12,Q16:Q26)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X28" s="4">
         <f>SUMPRODUCT(W2:W12,X16:X26)</f>

</xml_diff>